<commit_message>
Changes to accommodate BoM costs
</commit_message>
<xml_diff>
--- a/pH_meter_top_bom.xlsx
+++ b/pH_meter_top_bom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/51c118854276e9fd/Documents/GitHub/low_cost_pH_meter/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="36" documentId="8_{0DBDACE1-152B-4A7D-A7C7-E99FD8A029AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CFCA2746-3395-42EA-B327-3B6481F6EE1E}"/>
+  <xr:revisionPtr revIDLastSave="76" documentId="8_{0DBDACE1-152B-4A7D-A7C7-E99FD8A029AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4CDE70A8-8041-4395-A77B-013D3D1705F8}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F45CEF90-793B-493F-A039-0319F8578A82}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="95">
   <si>
     <t>Comment</t>
   </si>
@@ -118,15 +118,9 @@
     <t>PSON65P250X250X100-8N</t>
   </si>
   <si>
-    <t>LQW18AN2N2D10D</t>
-  </si>
-  <si>
     <t>L1</t>
   </si>
   <si>
-    <t>INDC1608X100N</t>
-  </si>
-  <si>
     <t>MIC5504-3.3YM5_TR</t>
   </si>
   <si>
@@ -163,15 +157,9 @@
     <t>QFN40P700X700X90-57N</t>
   </si>
   <si>
-    <t>SFH6325-X017T</t>
-  </si>
-  <si>
     <t>U5</t>
   </si>
   <si>
-    <t>SOIC254P1030X460-8N</t>
-  </si>
-  <si>
     <t>TF-123-ARP9HXX</t>
   </si>
   <si>
@@ -268,16 +256,55 @@
     <t>C2982548</t>
   </si>
   <si>
-    <t>C17481391</t>
-  </si>
-  <si>
     <t>C3021093</t>
   </si>
   <si>
     <t>C99271</t>
   </si>
   <si>
-    <t>C370207</t>
+    <t>C26413</t>
+  </si>
+  <si>
+    <t>C118155</t>
+  </si>
+  <si>
+    <t>C114662</t>
+  </si>
+  <si>
+    <t>C394543</t>
+  </si>
+  <si>
+    <t>C440186</t>
+  </si>
+  <si>
+    <t>C5250752</t>
+  </si>
+  <si>
+    <t>C658204</t>
+  </si>
+  <si>
+    <t>C92489</t>
+  </si>
+  <si>
+    <t>C465944</t>
+  </si>
+  <si>
+    <t>SOP-8</t>
+  </si>
+  <si>
+    <t>EL0631(TA)</t>
+  </si>
+  <si>
+    <t>LQW18AN2N2C80D</t>
+  </si>
+  <si>
+    <t>C71648</t>
+  </si>
+  <si>
+    <t>C3017771</t>
+  </si>
+  <si>
+    <t>C374544</t>
   </si>
 </sst>
 </file>
@@ -829,6 +856,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1151,7 +1182,7 @@
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1178,58 +1209,58 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C2">
         <v>603</v>
       </c>
       <c r="D2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B4" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30">
@@ -1243,7 +1274,7 @@
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1256,6 +1287,9 @@
       <c r="C7" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="D7" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
@@ -1267,6 +1301,9 @@
       <c r="C8" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="D8" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
@@ -1278,6 +1315,9 @@
       <c r="C9" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="D9" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
@@ -1289,6 +1329,9 @@
       <c r="C10" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="D10" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
@@ -1300,6 +1343,9 @@
       <c r="C11" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="D11" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
@@ -1312,7 +1358,7 @@
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.75">
@@ -1326,7 +1372,7 @@
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E13" s="3"/>
     </row>
@@ -1340,6 +1386,9 @@
       <c r="C14" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="D14" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
@@ -1351,6 +1400,9 @@
       <c r="C15" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="D15" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16">
@@ -1362,6 +1414,9 @@
       <c r="C16" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="D16" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17">
@@ -1371,10 +1426,10 @@
         <v>25</v>
       </c>
       <c r="C17" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D17" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1387,6 +1442,9 @@
       <c r="C18" t="s">
         <v>28</v>
       </c>
+      <c r="D18" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
@@ -1398,145 +1456,148 @@
       <c r="C19" t="s">
         <v>31</v>
       </c>
+      <c r="D19" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
+        <v>91</v>
+      </c>
+      <c r="B20" t="s">
         <v>32</v>
       </c>
-      <c r="B20" t="s">
-        <v>33</v>
-      </c>
       <c r="C20" t="s">
-        <v>34</v>
+        <v>91</v>
       </c>
       <c r="D20" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" t="s">
         <v>35</v>
       </c>
-      <c r="B21" t="s">
-        <v>36</v>
-      </c>
-      <c r="C21" t="s">
-        <v>37</v>
-      </c>
       <c r="D21" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" t="s">
         <v>38</v>
       </c>
-      <c r="B22" t="s">
-        <v>39</v>
-      </c>
-      <c r="C22" t="s">
-        <v>40</v>
-      </c>
       <c r="D22" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" t="s">
         <v>41</v>
       </c>
-      <c r="B23" t="s">
-        <v>42</v>
-      </c>
-      <c r="C23" t="s">
-        <v>43</v>
-      </c>
       <c r="D23" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" t="s">
         <v>44</v>
       </c>
-      <c r="B24" t="s">
-        <v>45</v>
-      </c>
-      <c r="C24" t="s">
-        <v>46</v>
-      </c>
       <c r="D24" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>47</v>
+        <v>90</v>
       </c>
       <c r="B25" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C25" t="s">
-        <v>49</v>
+        <v>89</v>
       </c>
       <c r="D25" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B26" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C26" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D26" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B27" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C27" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D27" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B28" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C28" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D28" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B29" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C29" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D29" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated gerber file checkin
Removed old gerber files
</commit_message>
<xml_diff>
--- a/pH_meter_top_bom.xlsx
+++ b/pH_meter_top_bom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/51c118854276e9fd/Documents/GitHub/low_cost_pH_meter/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="76" documentId="8_{0DBDACE1-152B-4A7D-A7C7-E99FD8A029AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4CDE70A8-8041-4395-A77B-013D3D1705F8}"/>
+  <xr:revisionPtr revIDLastSave="89" documentId="8_{0DBDACE1-152B-4A7D-A7C7-E99FD8A029AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5FE4BBC5-1801-4124-BAE8-9B7361F4679F}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F45CEF90-793B-493F-A039-0319F8578A82}"/>
+    <workbookView xWindow="-28920" yWindow="-30" windowWidth="29040" windowHeight="15720" xr2:uid="{F45CEF90-793B-493F-A039-0319F8578A82}"/>
   </bookViews>
   <sheets>
     <sheet name="pH_meter_top_bom" sheetId="1" r:id="rId1"/>
@@ -259,9 +259,6 @@
     <t>C3021093</t>
   </si>
   <si>
-    <t>C99271</t>
-  </si>
-  <si>
     <t>C26413</t>
   </si>
   <si>
@@ -305,6 +302,9 @@
   </si>
   <si>
     <t>C374544</t>
+  </si>
+  <si>
+    <t>C72443</t>
   </si>
 </sst>
 </file>
@@ -1182,7 +1182,7 @@
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1288,7 +1288,7 @@
         <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1302,7 +1302,7 @@
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1316,7 +1316,7 @@
         <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1330,7 +1330,7 @@
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1344,7 +1344,7 @@
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1387,7 +1387,7 @@
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1401,7 +1401,7 @@
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -1415,7 +1415,7 @@
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1443,7 +1443,7 @@
         <v>28</v>
       </c>
       <c r="D18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1457,21 +1457,21 @@
         <v>31</v>
       </c>
       <c r="D19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B20" t="s">
         <v>32</v>
       </c>
       <c r="C20" t="s">
+        <v>90</v>
+      </c>
+      <c r="D20" t="s">
         <v>91</v>
-      </c>
-      <c r="D20" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -1499,7 +1499,7 @@
         <v>38</v>
       </c>
       <c r="D22" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1532,16 +1532,16 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B25" t="s">
         <v>45</v>
       </c>
       <c r="C25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="26" spans="1:4">

</xml_diff>